<commit_message>
Control board wire harness directions
</commit_message>
<xml_diff>
--- a/Antonio-Feed/Wiring Harnesses/Feed/ Control Board to Cryo Board Cable (rainbow)/List of materials (rainbow).xlsx
+++ b/Antonio-Feed/Wiring Harnesses/Feed/ Control Board to Cryo Board Cable (rainbow)/List of materials (rainbow).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahschoultz/Documents/GitHub/Front-Page/Antonio-Feed/Wiring Harnesses/Feed/ Control Board to Cryo Board Cable (rainbow)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/Documents/Wiring Harness Directions/ Control Board to Cryo Board Cable (rainbow)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF9101E-F2D0-4F47-A923-14478FD69B0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FF1665-A8B4-EA41-937C-A7FE490BE5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="640" windowWidth="25440" windowHeight="14520" xr2:uid="{1354B1EE-61B1-EA40-838A-2C3EED4877E0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="103">
   <si>
     <t>Material</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Order Number of Distributor</t>
   </si>
   <si>
-    <t>Shrink tube</t>
-  </si>
-  <si>
     <t>Metal braid</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>Crimping D sub tips on</t>
   </si>
   <si>
-    <t>Metal extraction tool</t>
-  </si>
-  <si>
     <t xml:space="preserve">Attaching ground wire to metal braid </t>
   </si>
   <si>
@@ -295,23 +289,70 @@
   </si>
   <si>
     <t>Measuring lengths of materials</t>
+  </si>
+  <si>
+    <t>1/8 metal braid</t>
+  </si>
+  <si>
+    <t>Glenair</t>
+  </si>
+  <si>
+    <t>100-001A125</t>
+  </si>
+  <si>
+    <t>654-100001A125</t>
+  </si>
+  <si>
+    <t>4.8mm adhesive shrink tube</t>
+  </si>
+  <si>
+    <t>TE Connectivity / Raychem</t>
+  </si>
+  <si>
+    <t>TAT-125-3/16-0-STK</t>
+  </si>
+  <si>
+    <t>650-TAT125316</t>
+  </si>
+  <si>
+    <t>6.4mm in adehsive shrink tube</t>
+  </si>
+  <si>
+    <t>TAT-125-1/4-0-STK</t>
+  </si>
+  <si>
+    <t>650-TAT125014</t>
+  </si>
+  <si>
+    <t>16in</t>
+  </si>
+  <si>
+    <t>8in</t>
+  </si>
+  <si>
+    <t>7.25in</t>
+  </si>
+  <si>
+    <t>6.75in</t>
+  </si>
+  <si>
+    <t>1in</t>
+  </si>
+  <si>
+    <t>1.5in</t>
+  </si>
+  <si>
+    <t>Metal insertion tool</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -372,15 +413,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -704,7 +744,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:M3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -720,16 +760,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -741,10 +781,10 @@
       <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M1" s="3" t="s">
+      <c r="L1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -752,224 +792,251 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="C2" t="s">
+        <v>96</v>
+      </c>
       <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>59</v>
-      </c>
       <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
         <v>25</v>
-      </c>
-      <c r="M2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="7"/>
+      <c r="C3" t="s">
+        <v>96</v>
+      </c>
       <c r="D3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>60</v>
+        <v>55</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>61</v>
+        <v>46</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="L3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="C4" t="s">
+        <v>96</v>
+      </c>
       <c r="D4" t="s">
-        <v>57</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>62</v>
+        <v>55</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>63</v>
+        <v>46</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="L4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" t="s">
         <v>27</v>
-      </c>
-      <c r="M4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5" s="8"/>
+        <v>62</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" t="s">
+        <v>96</v>
+      </c>
       <c r="D5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>72</v>
+        <v>55</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" t="s">
         <v>29</v>
-      </c>
-      <c r="M5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="C6" t="s">
+        <v>96</v>
+      </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L6" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" t="s">
         <v>31</v>
-      </c>
-      <c r="M6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="7"/>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
       <c r="D7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>73</v>
+        <v>55</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="L7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="C8" t="s">
+        <v>96</v>
+      </c>
       <c r="D8" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>76</v>
+        <v>55</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="L8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="7"/>
+      <c r="C9" t="s">
+        <v>96</v>
+      </c>
       <c r="D9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>77</v>
+        <v>55</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L9" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" t="s">
         <v>34</v>
-      </c>
-      <c r="M9" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="7"/>
+      <c r="C10" t="s">
+        <v>96</v>
+      </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L10" t="s">
-        <v>36</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>44</v>
+        <v>35</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -979,133 +1046,184 @@
       <c r="B11" t="s">
         <v>15</v>
       </c>
+      <c r="C11" t="s">
+        <v>97</v>
+      </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L11" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" t="s">
+        <v>88</v>
+      </c>
+      <c r="L12" t="s">
         <v>37</v>
       </c>
-      <c r="M11" s="9"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>38</v>
-      </c>
-      <c r="M12" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>99</v>
       </c>
       <c r="D13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" t="s">
         <v>82</v>
       </c>
-      <c r="E13" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" t="s">
-        <v>84</v>
-      </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L13" t="s">
+        <v>39</v>
+      </c>
+      <c r="M13" t="s">
         <v>40</v>
       </c>
-      <c r="M13" t="s">
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" t="s">
+        <v>92</v>
+      </c>
+      <c r="L14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M14" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="M14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" t="s">
-        <v>21</v>
-      </c>
-      <c r="L15" s="5" t="s">
-        <v>43</v>
+      <c r="C15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" t="s">
+        <v>95</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>102</v>
       </c>
       <c r="M15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>53</v>
+      <c r="A16" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C16">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" t="s">
+        <v>49</v>
+      </c>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="F16" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" t="s">
-        <v>51</v>
-      </c>
-      <c r="L16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>52</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" t="s">
         <v>47</v>
-      </c>
-      <c r="F17" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>